<commit_message>
Actualizacion de repositio con clases de Ampliacion y Refinanciacion
</commit_message>
<xml_diff>
--- a/target/DatosExcel/DatosCreditoEmpresarialAmpliacion.xlsx
+++ b/target/DatosExcel/DatosCreditoEmpresarialAmpliacion.xlsx
@@ -3,20 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CMACPiura_2022\target\DatosExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4545"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Cliente</t>
   </si>
@@ -47,21 +47,42 @@
     <t>Tipo Operación</t>
   </si>
   <si>
+    <t>Pagaré</t>
+  </si>
+  <si>
     <t>Monto</t>
   </si>
   <si>
+    <t>Tasa Inicial Pricing</t>
+  </si>
+  <si>
     <t>Plan Pagos</t>
   </si>
   <si>
     <t>Modalidad Amortizacion</t>
   </si>
   <si>
+    <t>Opción Pago</t>
+  </si>
+  <si>
+    <t>Día Pago</t>
+  </si>
+  <si>
+    <t>Número Cuotas</t>
+  </si>
+  <si>
     <t>Tasa Preferencial</t>
   </si>
   <si>
     <t>Forma Desembolso</t>
   </si>
   <si>
+    <t>Observacion Notas</t>
+  </si>
+  <si>
+    <t>Observaciones dictamen</t>
+  </si>
+  <si>
     <t>Contraseña</t>
   </si>
   <si>
@@ -77,9 +98,15 @@
     <t>CREDITOS PYMES</t>
   </si>
   <si>
+    <t>AMPLIACION</t>
+  </si>
+  <si>
     <t>NORMAL</t>
   </si>
   <si>
+    <t>CREDITO AL TOQUE</t>
+  </si>
+  <si>
     <t>SIMPLE</t>
   </si>
   <si>
@@ -89,80 +116,49 @@
     <t>Fija Vencida</t>
   </si>
   <si>
+    <t>Cronograma Pagos</t>
+  </si>
+  <si>
+    <t>Fecha Fija</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>36.05</t>
+  </si>
+  <si>
+    <t>ABONO EN CUENTA</t>
+  </si>
+  <si>
+    <t>Prueba Ampliacion</t>
+  </si>
+  <si>
+    <t>Aprobar Ampliacion</t>
+  </si>
+  <si>
     <t>prueba</t>
   </si>
   <si>
-    <t>AMPLIACION</t>
-  </si>
-  <si>
-    <t>CREDITO AL TOQUE</t>
-  </si>
-  <si>
-    <t>Pagaré</t>
-  </si>
-  <si>
-    <t>080-01-9847672</t>
-  </si>
-  <si>
-    <t>Tasa Inicial Pricing</t>
-  </si>
-  <si>
-    <t>5000</t>
-  </si>
-  <si>
-    <t>Cronograma Pagos</t>
-  </si>
-  <si>
-    <t>Opción Pago</t>
-  </si>
-  <si>
-    <t>Fecha Fija</t>
-  </si>
-  <si>
-    <t>Día Pago</t>
-  </si>
-  <si>
-    <t>Número Cuotas</t>
-  </si>
-  <si>
-    <t>18919826</t>
-  </si>
-  <si>
-    <t>ABONO EN CUENTA</t>
-  </si>
-  <si>
-    <t>Observacion Notas</t>
-  </si>
-  <si>
-    <t>Prueba Ampliacion</t>
-  </si>
-  <si>
-    <t>36.05</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>Observaciones dictamen</t>
-  </si>
-  <si>
-    <t>Aprobar Ampliacion</t>
-  </si>
-  <si>
-    <t>4978693</t>
-  </si>
-  <si>
-    <t>Se han encontrado errores en la Validacion de la Propuesta</t>
+    <t>Resultado con ADN</t>
+  </si>
+  <si>
+    <t>23770571</t>
+  </si>
+  <si>
+    <t>080-01-0456093</t>
+  </si>
+  <si>
+    <t>2000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -510,28 +506,21 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="29.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" style="1" width="12.0" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="27.7109375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="23.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="31.85546875" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" width="27.0" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" width="26.28515625" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" width="45.42578125" collapsed="true"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="54" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
@@ -557,124 +546,126 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27">
       <c r="A2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>39</v>
-      </c>
       <c r="P2" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>36</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="U2" t="s">
-        <v>42</v>
-      </c>
-      <c r="V2" t="s">
-        <v>43</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
       <c r="W2" s="3"/>
       <c r="X2" s="3"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27">
       <c r="C3" s="1"/>
@@ -688,17 +679,16 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
-      <c r="AA3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>